<commit_message>
Changed Gantt Start Date and Added Milestones
</commit_message>
<xml_diff>
--- a/Native/CougSat1-Timeline.xlsx
+++ b/Native/CougSat1-Timeline.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bradley\Documents\GitHub\CougSat1-Readme\Native\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A9D7B42-3DBE-40F4-BBBE-1D334D903F6E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{987F3A74-B9D5-4D4F-B621-4C7B3ED53191}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7485" xr2:uid="{6C898573-EEE6-4764-A1E5-48C0D9787F59}"/>
   </bookViews>
   <sheets>
     <sheet name="Text" sheetId="7" r:id="rId1"/>
     <sheet name="Gantt" sheetId="8" r:id="rId2"/>
+    <sheet name="Gantt Lines" sheetId="9" state="hidden" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="Design">Text!$E$4:$E$22</definedName>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="62">
   <si>
     <t>Start</t>
   </si>
@@ -144,9 +145,6 @@
     <t>End:</t>
   </si>
   <si>
-    <t>Start:</t>
-  </si>
-  <si>
     <t>Implement Part 1</t>
   </si>
   <si>
@@ -177,7 +175,61 @@
     <t>Self-contained system within the satellite</t>
   </si>
   <si>
-    <t>V1.1.0</t>
+    <t>Milestones</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>EM Integration</t>
+  </si>
+  <si>
+    <t>FRR</t>
+  </si>
+  <si>
+    <t>MRR</t>
+  </si>
+  <si>
+    <t>ILC</t>
+  </si>
+  <si>
+    <t>FU Day in the Life Test</t>
+  </si>
+  <si>
+    <t>EM Day in the Life Test</t>
+  </si>
+  <si>
+    <t>FU Integration</t>
+  </si>
+  <si>
+    <t>Initial launch capabilities</t>
+  </si>
+  <si>
+    <t>A duration test of the satellite in simulated space environment. Requires: all software done</t>
+  </si>
+  <si>
+    <t>Assembly of all subsystems and components. Requires: all hardware done</t>
+  </si>
+  <si>
+    <t>Assembly of all flight ready subsystems and components</t>
+  </si>
+  <si>
+    <t>A duration test of the flight unit in simulated space environment</t>
+  </si>
+  <si>
+    <t>Review of the flight unit to determine its readiness to fly</t>
+  </si>
+  <si>
+    <t>Review of the mission to determine its readiness to execute</t>
+  </si>
+  <si>
+    <t>V1.1.1</t>
   </si>
 </sst>
 </file>
@@ -368,7 +420,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -554,6 +606,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -561,7 +641,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -570,14 +650,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="17" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="7" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -593,9 +668,6 @@
     <xf numFmtId="0" fontId="7" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="17" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="7" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -609,9 +681,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="17" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="7" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -693,12 +762,24 @@
     <xf numFmtId="0" fontId="4" fillId="15" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="4" fillId="15" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -720,18 +801,6 @@
     <xf numFmtId="164" fontId="9" fillId="3" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -740,6 +809,41 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="15" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="17" borderId="17" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="17" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="17" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="17" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="15" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="15" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="15" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="16" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="17" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1082,7 +1186,7 @@
                   <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>14</c:v>
@@ -1124,10 +1228,10 @@
                   <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>14</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>14</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>21</c:v>
@@ -1284,7 +1388,7 @@
                   <c:v>280</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>49</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>56</c:v>
@@ -1299,7 +1403,7 @@
                   <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>49</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>49</c:v>
@@ -1323,7 +1427,7 @@
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>98</c:v>
+                  <c:v>154</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>28</c:v>
@@ -1467,13 +1571,13 @@
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>77</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>28</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>21</c:v>
@@ -1503,10 +1607,10 @@
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>98</c:v>
+                  <c:v>112</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>28</c:v>
@@ -1647,13 +1751,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>56</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>21</c:v>
@@ -1725,6 +1829,524 @@
         <c:axId val="413356223"/>
         <c:axId val="295186255"/>
       </c:barChart>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Gantt Lines'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Today: 28-Oct-18</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Gantt Lines'!$A$2:$A$3</c:f>
+              <c:numCache>
+                <c:formatCode>[$-409]d\-mmm\-yy;@</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>43401</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43401</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Gantt Lines'!$B$2:$B$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-BB20-477D-9AD2-367277961686}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Gantt Lines'!$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>EM Integration</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Gantt Lines'!$A$6:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>43522</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43522</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Gantt Lines'!$B$6:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-BB20-477D-9AD2-367277961686}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Gantt Lines'!$B$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>EM Day in the Life Test</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Gantt Lines'!$A$10:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>43578</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43578</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Gantt Lines'!$B$10:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-BB20-477D-9AD2-367277961686}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Gantt Lines'!$B$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FU Integration</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Gantt Lines'!$A$14:$A$15</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>43620</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43620</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Gantt Lines'!$B$14:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-BB20-477D-9AD2-367277961686}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Gantt Lines'!$B$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FU Day in the Life Test</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Gantt Lines'!$A$18:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>43648</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43648</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Gantt Lines'!$B$18:$B$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-BB20-477D-9AD2-367277961686}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Gantt Lines'!$B$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FRR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Gantt Lines'!$A$22:$A$23</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>43662</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43662</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Gantt Lines'!$B$22:$B$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-BB20-477D-9AD2-367277961686}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="11"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Gantt Lines'!$B$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MRR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Gantt Lines'!$A$26:$A$27</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>43676</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43676</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Gantt Lines'!$B$26:$B$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-BB20-477D-9AD2-367277961686}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="12"/>
+          <c:order val="12"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Gantt Lines'!$B$29</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ILC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="00B0F0"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Gantt Lines'!$A$30:$A$31</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>43690</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43690</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Gantt Lines'!$B$30:$B$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000C-BB20-477D-9AD2-367277961686}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="226793872"/>
+        <c:axId val="2047381920"/>
+      </c:scatterChart>
       <c:catAx>
         <c:axId val="413356223"/>
         <c:scaling>
@@ -1780,8 +2402,8 @@
         <c:axId val="295186255"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="43669"/>
-          <c:min val="43221"/>
+          <c:max val="43816"/>
+          <c:min val="43396"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="t"/>
@@ -1849,6 +2471,62 @@
         <c:crossBetween val="between"/>
         <c:majorUnit val="28"/>
         <c:minorUnit val="7"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2047381920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="none"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="226793872"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="226793872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="[$-409]d\-mmm\-yy;@" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2047381920"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -2489,7 +3167,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="12239625" cy="7210425"/>
+    <xdr:ext cx="11858625" cy="7191375"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -2815,10 +3493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6795B2AF-B69F-4446-A3B6-FEFF9CA8AA9F}">
-  <dimension ref="A1:P25"/>
+  <dimension ref="A1:P31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:F2"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2827,312 +3505,309 @@
     <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" style="32" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" style="27" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" style="32" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" style="27" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" style="32" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" style="27" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.85546875" style="32" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" style="27" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="24.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="47" t="s">
-        <v>44</v>
-      </c>
-      <c r="F1" s="48" t="s">
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="43"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="50">
+        <f>L5</f>
+        <v>43690</v>
+      </c>
+      <c r="L1" s="51"/>
+    </row>
+    <row r="2" spans="1:16" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="46"/>
+      <c r="G2" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="51">
-        <f>D4</f>
-        <v>43221</v>
-      </c>
-      <c r="H1" s="53"/>
-      <c r="I1" s="47">
-        <f>(K1-G1)/7</f>
-        <v>64</v>
-      </c>
-      <c r="J1" s="48" t="s">
-        <v>32</v>
-      </c>
-      <c r="K1" s="51">
-        <f>L5</f>
-        <v>43669</v>
-      </c>
-      <c r="L1" s="52"/>
-    </row>
-    <row r="2" spans="1:16" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="43" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="43" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="59" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="59"/>
-      <c r="G2" s="60" t="s">
+      <c r="H2" s="47"/>
+      <c r="I2" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="60"/>
-      <c r="I2" s="61" t="s">
+      <c r="J2" s="48"/>
+      <c r="K2" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" s="57"/>
+    </row>
+    <row r="3" spans="1:16" s="5" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="53" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="53"/>
+      <c r="G3" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="54"/>
+      <c r="I3" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="J2" s="61"/>
-      <c r="K2" s="62" t="s">
-        <v>4</v>
-      </c>
-      <c r="L2" s="62"/>
-    </row>
-    <row r="3" spans="1:16" s="5" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="45" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3" s="45" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3" s="54" t="s">
-        <v>42</v>
-      </c>
-      <c r="F3" s="54"/>
-      <c r="G3" s="55" t="s">
+      <c r="J3" s="55"/>
+      <c r="K3" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="H3" s="55"/>
-      <c r="I3" s="56" t="s">
-        <v>36</v>
-      </c>
-      <c r="J3" s="56"/>
-      <c r="K3" s="57" t="s">
-        <v>38</v>
-      </c>
-      <c r="L3" s="57"/>
+      <c r="L3" s="56"/>
+      <c r="M3" s="60"/>
     </row>
     <row r="4" spans="1:16" ht="21.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="61">
         <v>43221</v>
       </c>
-      <c r="E4" s="29">
+      <c r="E4" s="24">
         <f>(F4-D4)/7</f>
         <v>3</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="7">
         <f>MIN(D6:D22)</f>
         <v>43242</v>
       </c>
-      <c r="G4" s="33">
+      <c r="G4" s="28">
         <f>(H4-F4)/7</f>
         <v>40</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H4" s="8">
         <f>_xlfn.MAXIFS(L6:L22,C6:C22,"Hardware")</f>
         <v>43522</v>
       </c>
-      <c r="I4" s="36">
+      <c r="I4" s="31">
         <v>2</v>
       </c>
-      <c r="J4" s="12">
+      <c r="J4" s="9">
         <f>H4+I4*7</f>
         <v>43536</v>
       </c>
-      <c r="K4" s="39">
-        <v>4</v>
-      </c>
-      <c r="L4" s="13">
-        <f>J4+K4*7</f>
-        <v>43564</v>
-      </c>
+      <c r="K4" s="34">
+        <f>(L4-J4)/7</f>
+        <v>8</v>
+      </c>
+      <c r="L4" s="10">
+        <f>MAX(L6:L22)+14</f>
+        <v>43592</v>
+      </c>
+      <c r="M4" s="2"/>
     </row>
     <row r="5" spans="1:16" ht="21" x14ac:dyDescent="0.25">
-      <c r="A5" s="50"/>
-      <c r="B5" s="42" t="s">
+      <c r="A5" s="45"/>
+      <c r="B5" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="62">
         <f>J4</f>
         <v>43536</v>
       </c>
-      <c r="E5" s="30">
-        <v>2</v>
-      </c>
-      <c r="F5" s="16">
-        <f>D5+E5*7</f>
-        <v>43550</v>
-      </c>
-      <c r="G5" s="34">
-        <v>7</v>
-      </c>
-      <c r="H5" s="17">
+      <c r="E5" s="25">
+        <f>(F5-D5)/7</f>
+        <v>8</v>
+      </c>
+      <c r="F5" s="12">
+        <f>L4</f>
+        <v>43592</v>
+      </c>
+      <c r="G5" s="29">
+        <v>4</v>
+      </c>
+      <c r="H5" s="13">
         <f>F5+G5*7</f>
-        <v>43599</v>
-      </c>
-      <c r="I5" s="37">
-        <v>2</v>
-      </c>
-      <c r="J5" s="18">
+        <v>43620</v>
+      </c>
+      <c r="I5" s="32">
+        <v>4</v>
+      </c>
+      <c r="J5" s="14">
         <f>H5+I5*7</f>
-        <v>43613</v>
-      </c>
-      <c r="K5" s="40">
-        <v>8</v>
-      </c>
-      <c r="L5" s="19">
-        <f>J5+K5*7</f>
-        <v>43669</v>
+        <v>43648</v>
+      </c>
+      <c r="K5" s="35">
+        <f>(L5-J5)/7</f>
+        <v>6</v>
+      </c>
+      <c r="L5" s="15">
+        <f>L31</f>
+        <v>43690</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="63">
         <v>43242</v>
       </c>
-      <c r="E6" s="29">
+      <c r="E6" s="24">
         <v>2</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="7">
         <f>D6+E6*7</f>
         <v>43256</v>
       </c>
-      <c r="G6" s="33">
+      <c r="G6" s="28">
         <v>8</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="8">
         <f>F6+G6*7</f>
         <v>43312</v>
       </c>
-      <c r="I6" s="36">
+      <c r="I6" s="31">
         <v>11</v>
       </c>
-      <c r="J6" s="12">
+      <c r="J6" s="9">
         <f>H6+I6*7</f>
         <v>43389</v>
       </c>
-      <c r="K6" s="39">
-        <v>3</v>
-      </c>
-      <c r="L6" s="13">
+      <c r="K6" s="34">
+        <v>4</v>
+      </c>
+      <c r="L6" s="10">
         <f>J6+K6*7</f>
-        <v>43410</v>
+        <v>43417</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="49"/>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="63">
         <v>43312</v>
       </c>
-      <c r="E7" s="29">
+      <c r="E7" s="24">
         <v>2</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="7">
         <f t="shared" ref="F7:F22" si="0">D7+E7*7</f>
         <v>43326</v>
       </c>
-      <c r="G7" s="33">
+      <c r="G7" s="28">
         <v>8</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="8">
         <f t="shared" ref="H7:H22" si="1">F7+G7*7</f>
         <v>43382</v>
       </c>
-      <c r="I7" s="36">
-        <v>4</v>
-      </c>
-      <c r="J7" s="12">
+      <c r="I7" s="31">
+        <v>5</v>
+      </c>
+      <c r="J7" s="9">
         <f t="shared" ref="J7:J22" si="2">H7+I7*7</f>
-        <v>43410</v>
-      </c>
-      <c r="K7" s="39">
+        <v>43417</v>
+      </c>
+      <c r="K7" s="34">
         <v>3</v>
       </c>
-      <c r="L7" s="13">
+      <c r="L7" s="10">
         <f t="shared" ref="L7:L22" si="3">J7+K7*7</f>
-        <v>43431</v>
+        <v>43438</v>
       </c>
       <c r="O7" s="3"/>
       <c r="P7" s="2"/>
     </row>
     <row r="8" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="49"/>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="63">
         <v>43340</v>
       </c>
-      <c r="E8" s="29">
+      <c r="E8" s="24">
         <v>2</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="7">
         <f t="shared" si="0"/>
         <v>43354</v>
       </c>
-      <c r="G8" s="33">
+      <c r="G8" s="28">
         <v>3</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H8" s="8">
         <f t="shared" si="1"/>
         <v>43375</v>
       </c>
-      <c r="I8" s="36">
+      <c r="I8" s="31">
         <v>3</v>
       </c>
-      <c r="J8" s="12">
+      <c r="J8" s="9">
         <f t="shared" si="2"/>
         <v>43396</v>
       </c>
-      <c r="K8" s="39">
+      <c r="K8" s="34">
         <v>3</v>
       </c>
-      <c r="L8" s="13">
+      <c r="L8" s="10">
         <f t="shared" si="3"/>
         <v>43417</v>
       </c>
@@ -3140,582 +3815,785 @@
       <c r="P8" s="2"/>
     </row>
     <row r="9" spans="1:16" ht="21" x14ac:dyDescent="0.25">
-      <c r="A9" s="50"/>
-      <c r="B9" s="14" t="s">
+      <c r="A9" s="45"/>
+      <c r="B9" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="62">
         <v>43396</v>
       </c>
-      <c r="E9" s="30">
+      <c r="E9" s="25">
         <v>3</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9" s="12">
         <f t="shared" si="0"/>
         <v>43417</v>
       </c>
-      <c r="G9" s="34">
+      <c r="G9" s="29">
         <v>8</v>
       </c>
-      <c r="H9" s="17">
+      <c r="H9" s="13">
         <f t="shared" si="1"/>
         <v>43473</v>
       </c>
-      <c r="I9" s="37">
+      <c r="I9" s="32">
         <v>3</v>
       </c>
-      <c r="J9" s="18">
+      <c r="J9" s="14">
         <f t="shared" si="2"/>
         <v>43494</v>
       </c>
-      <c r="K9" s="40">
+      <c r="K9" s="35">
         <v>3</v>
       </c>
-      <c r="L9" s="19">
+      <c r="L9" s="15">
         <f t="shared" si="3"/>
         <v>43515</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="21" x14ac:dyDescent="0.25">
-      <c r="A10" s="58" t="s">
+      <c r="A10" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="21">
+      <c r="D10" s="64">
         <v>43340</v>
       </c>
-      <c r="E10" s="31">
+      <c r="E10" s="26">
         <v>3</v>
       </c>
-      <c r="F10" s="22">
+      <c r="F10" s="17">
         <f t="shared" si="0"/>
         <v>43361</v>
       </c>
-      <c r="G10" s="35">
+      <c r="G10" s="30">
+        <v>8</v>
+      </c>
+      <c r="H10" s="18">
+        <f t="shared" si="1"/>
+        <v>43417</v>
+      </c>
+      <c r="I10" s="33">
         <v>7</v>
       </c>
-      <c r="H10" s="23">
+      <c r="J10" s="19">
+        <f t="shared" si="2"/>
+        <v>43466</v>
+      </c>
+      <c r="K10" s="36">
+        <v>3</v>
+      </c>
+      <c r="L10" s="20">
+        <f t="shared" si="3"/>
+        <v>43487</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A11" s="49"/>
+      <c r="B11" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="63">
+        <v>43368</v>
+      </c>
+      <c r="E11" s="24">
+        <v>7</v>
+      </c>
+      <c r="F11" s="7">
+        <f t="shared" si="0"/>
+        <v>43417</v>
+      </c>
+      <c r="G11" s="28">
+        <v>7</v>
+      </c>
+      <c r="H11" s="8">
+        <f t="shared" si="1"/>
+        <v>43466</v>
+      </c>
+      <c r="I11" s="31">
+        <v>3</v>
+      </c>
+      <c r="J11" s="9">
+        <f t="shared" si="2"/>
+        <v>43487</v>
+      </c>
+      <c r="K11" s="34">
+        <v>7</v>
+      </c>
+      <c r="L11" s="10">
+        <f t="shared" si="3"/>
+        <v>43536</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A12" s="49"/>
+      <c r="B12" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="63">
+        <v>43417</v>
+      </c>
+      <c r="E12" s="24">
+        <v>3</v>
+      </c>
+      <c r="F12" s="7">
+        <f t="shared" si="0"/>
+        <v>43438</v>
+      </c>
+      <c r="G12" s="28">
+        <v>7</v>
+      </c>
+      <c r="H12" s="8">
+        <f t="shared" si="1"/>
+        <v>43487</v>
+      </c>
+      <c r="I12" s="31">
+        <v>3</v>
+      </c>
+      <c r="J12" s="9">
+        <f t="shared" si="2"/>
+        <v>43508</v>
+      </c>
+      <c r="K12" s="34">
+        <v>7</v>
+      </c>
+      <c r="L12" s="10">
+        <f t="shared" si="3"/>
+        <v>43557</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A13" s="45"/>
+      <c r="B13" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="62">
+        <v>43368</v>
+      </c>
+      <c r="E13" s="25">
+        <v>3</v>
+      </c>
+      <c r="F13" s="12">
+        <f t="shared" si="0"/>
+        <v>43389</v>
+      </c>
+      <c r="G13" s="29">
+        <v>11</v>
+      </c>
+      <c r="H13" s="13">
+        <f t="shared" si="1"/>
+        <v>43466</v>
+      </c>
+      <c r="I13" s="32">
+        <v>3</v>
+      </c>
+      <c r="J13" s="14">
+        <f t="shared" si="2"/>
+        <v>43487</v>
+      </c>
+      <c r="K13" s="35">
+        <v>7</v>
+      </c>
+      <c r="L13" s="15">
+        <f t="shared" si="3"/>
+        <v>43536</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A14" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="64">
+        <v>43340</v>
+      </c>
+      <c r="E14" s="26">
+        <v>7</v>
+      </c>
+      <c r="F14" s="17">
+        <f t="shared" si="0"/>
+        <v>43389</v>
+      </c>
+      <c r="G14" s="30">
+        <v>8</v>
+      </c>
+      <c r="H14" s="18">
+        <f t="shared" si="1"/>
+        <v>43445</v>
+      </c>
+      <c r="I14" s="33">
+        <v>8</v>
+      </c>
+      <c r="J14" s="19">
+        <f t="shared" si="2"/>
+        <v>43501</v>
+      </c>
+      <c r="K14" s="36">
+        <v>3</v>
+      </c>
+      <c r="L14" s="20">
+        <f t="shared" si="3"/>
+        <v>43522</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A15" s="49"/>
+      <c r="B15" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="63">
+        <v>43417</v>
+      </c>
+      <c r="E15" s="24">
+        <v>7</v>
+      </c>
+      <c r="F15" s="7">
+        <f t="shared" si="0"/>
+        <v>43466</v>
+      </c>
+      <c r="G15" s="28">
+        <v>3</v>
+      </c>
+      <c r="H15" s="8">
+        <f t="shared" si="1"/>
+        <v>43487</v>
+      </c>
+      <c r="I15" s="31">
+        <v>6</v>
+      </c>
+      <c r="J15" s="9">
+        <f t="shared" si="2"/>
+        <v>43529</v>
+      </c>
+      <c r="K15" s="34">
+        <v>7</v>
+      </c>
+      <c r="L15" s="10">
+        <f t="shared" si="3"/>
+        <v>43578</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A16" s="49"/>
+      <c r="B16" s="6" t="str">
+        <f>"+X Panel"</f>
+        <v>+X Panel</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="63">
+        <v>43368</v>
+      </c>
+      <c r="E16" s="24">
+        <v>3</v>
+      </c>
+      <c r="F16" s="7">
+        <f t="shared" si="0"/>
+        <v>43389</v>
+      </c>
+      <c r="G16" s="28">
+        <v>2</v>
+      </c>
+      <c r="H16" s="8">
+        <f t="shared" si="1"/>
+        <v>43403</v>
+      </c>
+      <c r="I16" s="31">
+        <v>2</v>
+      </c>
+      <c r="J16" s="9">
+        <f t="shared" si="2"/>
+        <v>43417</v>
+      </c>
+      <c r="K16" s="34">
+        <v>3</v>
+      </c>
+      <c r="L16" s="10">
+        <f t="shared" si="3"/>
+        <v>43438</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="21" x14ac:dyDescent="0.25">
+      <c r="A17" s="49"/>
+      <c r="B17" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="63">
+        <v>43340</v>
+      </c>
+      <c r="E17" s="24">
+        <v>8</v>
+      </c>
+      <c r="F17" s="7">
+        <f t="shared" si="0"/>
+        <v>43396</v>
+      </c>
+      <c r="G17" s="28">
+        <v>2</v>
+      </c>
+      <c r="H17" s="8">
         <f t="shared" si="1"/>
         <v>43410</v>
       </c>
-      <c r="I10" s="38">
+      <c r="I17" s="31">
+        <v>2</v>
+      </c>
+      <c r="J17" s="9">
+        <f t="shared" si="2"/>
+        <v>43424</v>
+      </c>
+      <c r="K17" s="34">
+        <v>3</v>
+      </c>
+      <c r="L17" s="10">
+        <f t="shared" si="3"/>
+        <v>43445</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="21" x14ac:dyDescent="0.25">
+      <c r="A18" s="45"/>
+      <c r="B18" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="62">
+        <v>43242</v>
+      </c>
+      <c r="E18" s="25">
+        <v>3</v>
+      </c>
+      <c r="F18" s="12">
+        <f t="shared" si="0"/>
+        <v>43263</v>
+      </c>
+      <c r="G18" s="29">
+        <v>22</v>
+      </c>
+      <c r="H18" s="13">
+        <f t="shared" si="1"/>
+        <v>43417</v>
+      </c>
+      <c r="I18" s="32">
+        <v>16</v>
+      </c>
+      <c r="J18" s="14">
+        <f t="shared" si="2"/>
+        <v>43529</v>
+      </c>
+      <c r="K18" s="35">
         <v>7</v>
       </c>
-      <c r="J10" s="24">
-        <f t="shared" si="2"/>
-        <v>43459</v>
-      </c>
-      <c r="K10" s="41">
+      <c r="L18" s="15">
+        <f t="shared" si="3"/>
+        <v>43578</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="21" x14ac:dyDescent="0.25">
+      <c r="A19" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="64">
+        <v>43396</v>
+      </c>
+      <c r="E19" s="26">
         <v>3</v>
       </c>
-      <c r="L10" s="25">
-        <f t="shared" si="3"/>
-        <v>43480</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="49"/>
-      <c r="B11" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="9">
-        <v>43368</v>
-      </c>
-      <c r="E11" s="29">
-        <v>7</v>
-      </c>
-      <c r="F11" s="10">
+      <c r="F19" s="17">
         <f t="shared" si="0"/>
         <v>43417</v>
       </c>
-      <c r="G11" s="33">
-        <v>7</v>
-      </c>
-      <c r="H11" s="11">
-        <f t="shared" si="1"/>
-        <v>43466</v>
-      </c>
-      <c r="I11" s="36">
-        <v>3</v>
-      </c>
-      <c r="J11" s="12">
-        <f t="shared" si="2"/>
-        <v>43487</v>
-      </c>
-      <c r="K11" s="39">
-        <v>7</v>
-      </c>
-      <c r="L11" s="13">
-        <f t="shared" si="3"/>
-        <v>43536</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="49"/>
-      <c r="B12" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="9">
-        <v>43417</v>
-      </c>
-      <c r="E12" s="29">
-        <v>3</v>
-      </c>
-      <c r="F12" s="10">
-        <f t="shared" si="0"/>
-        <v>43438</v>
-      </c>
-      <c r="G12" s="33">
-        <v>7</v>
-      </c>
-      <c r="H12" s="11">
-        <f t="shared" si="1"/>
-        <v>43487</v>
-      </c>
-      <c r="I12" s="36">
-        <v>3</v>
-      </c>
-      <c r="J12" s="12">
-        <f t="shared" si="2"/>
-        <v>43508</v>
-      </c>
-      <c r="K12" s="39">
-        <v>7</v>
-      </c>
-      <c r="L12" s="13">
-        <f t="shared" si="3"/>
-        <v>43557</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" ht="21" x14ac:dyDescent="0.25">
-      <c r="A13" s="50"/>
-      <c r="B13" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" s="15">
-        <v>43368</v>
-      </c>
-      <c r="E13" s="30">
-        <v>3</v>
-      </c>
-      <c r="F13" s="16">
-        <f t="shared" si="0"/>
-        <v>43389</v>
-      </c>
-      <c r="G13" s="34">
-        <v>11</v>
-      </c>
-      <c r="H13" s="17">
-        <f t="shared" si="1"/>
-        <v>43466</v>
-      </c>
-      <c r="I13" s="37">
-        <v>3</v>
-      </c>
-      <c r="J13" s="18">
-        <f t="shared" si="2"/>
-        <v>43487</v>
-      </c>
-      <c r="K13" s="40">
-        <v>7</v>
-      </c>
-      <c r="L13" s="19">
-        <f t="shared" si="3"/>
-        <v>43536</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" ht="21" x14ac:dyDescent="0.25">
-      <c r="A14" s="58" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="21">
-        <v>43340</v>
-      </c>
-      <c r="E14" s="31">
-        <v>7</v>
-      </c>
-      <c r="F14" s="22">
-        <f t="shared" si="0"/>
-        <v>43389</v>
-      </c>
-      <c r="G14" s="35">
-        <v>8</v>
-      </c>
-      <c r="H14" s="23">
+      <c r="G19" s="30">
+        <v>4</v>
+      </c>
+      <c r="H19" s="18">
         <f t="shared" si="1"/>
         <v>43445</v>
       </c>
-      <c r="I14" s="38">
-        <v>8</v>
-      </c>
-      <c r="J14" s="24">
+      <c r="I19" s="33">
+        <v>4</v>
+      </c>
+      <c r="J19" s="19">
         <f t="shared" si="2"/>
-        <v>43501</v>
-      </c>
-      <c r="K14" s="41">
+        <v>43473</v>
+      </c>
+      <c r="K19" s="36">
         <v>3</v>
       </c>
-      <c r="L14" s="25">
+      <c r="L19" s="20">
         <f t="shared" si="3"/>
-        <v>43522</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="49"/>
-      <c r="B15" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="9">
+        <v>43494</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="21" x14ac:dyDescent="0.25">
+      <c r="A20" s="45"/>
+      <c r="B20" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="62">
+        <v>43396</v>
+      </c>
+      <c r="E20" s="25">
+        <v>3</v>
+      </c>
+      <c r="F20" s="12">
+        <f t="shared" si="0"/>
         <v>43417</v>
       </c>
-      <c r="E15" s="29">
+      <c r="G20" s="29">
+        <v>4</v>
+      </c>
+      <c r="H20" s="13">
+        <f t="shared" si="1"/>
+        <v>43445</v>
+      </c>
+      <c r="I20" s="32">
+        <v>4</v>
+      </c>
+      <c r="J20" s="14">
+        <f t="shared" si="2"/>
+        <v>43473</v>
+      </c>
+      <c r="K20" s="35">
+        <v>3</v>
+      </c>
+      <c r="L20" s="15">
+        <f t="shared" si="3"/>
+        <v>43494</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="21" x14ac:dyDescent="0.25">
+      <c r="A21" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="63">
+        <v>43242</v>
+      </c>
+      <c r="E21" s="24">
+        <v>3</v>
+      </c>
+      <c r="F21" s="7">
+        <f t="shared" si="0"/>
+        <v>43263</v>
+      </c>
+      <c r="G21" s="28">
+        <v>14</v>
+      </c>
+      <c r="H21" s="8">
+        <f t="shared" si="1"/>
+        <v>43361</v>
+      </c>
+      <c r="I21" s="31">
         <v>7</v>
       </c>
-      <c r="F15" s="10">
+      <c r="J21" s="9">
+        <f t="shared" si="2"/>
+        <v>43410</v>
+      </c>
+      <c r="K21" s="34">
+        <v>3</v>
+      </c>
+      <c r="L21" s="10">
+        <f t="shared" si="3"/>
+        <v>43431</v>
+      </c>
+      <c r="M21" s="4"/>
+    </row>
+    <row r="22" spans="1:13" ht="21" x14ac:dyDescent="0.25">
+      <c r="A22" s="45"/>
+      <c r="B22" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="62">
+        <v>43242</v>
+      </c>
+      <c r="E22" s="25">
+        <v>7</v>
+      </c>
+      <c r="F22" s="12">
         <f t="shared" si="0"/>
-        <v>43466</v>
-      </c>
-      <c r="G15" s="33">
-        <v>3</v>
-      </c>
-      <c r="H15" s="11">
+        <v>43291</v>
+      </c>
+      <c r="G22" s="29">
+        <v>11</v>
+      </c>
+      <c r="H22" s="13">
         <f t="shared" si="1"/>
-        <v>43487</v>
-      </c>
-      <c r="I15" s="36">
-        <v>6</v>
-      </c>
-      <c r="J15" s="12">
-        <f t="shared" si="2"/>
-        <v>43529</v>
-      </c>
-      <c r="K15" s="39">
+        <v>43368</v>
+      </c>
+      <c r="I22" s="32">
         <v>7</v>
       </c>
-      <c r="L15" s="13">
-        <f t="shared" si="3"/>
-        <v>43578</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" ht="21" x14ac:dyDescent="0.25">
-      <c r="A16" s="49"/>
-      <c r="B16" s="8" t="str">
-        <f>"+X Panel"</f>
-        <v>+X Panel</v>
-      </c>
-      <c r="C16" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="9">
-        <v>43368</v>
-      </c>
-      <c r="E16" s="29">
-        <v>3</v>
-      </c>
-      <c r="F16" s="10">
-        <f t="shared" si="0"/>
-        <v>43389</v>
-      </c>
-      <c r="G16" s="33">
-        <v>2</v>
-      </c>
-      <c r="H16" s="11">
-        <f t="shared" si="1"/>
-        <v>43403</v>
-      </c>
-      <c r="I16" s="36">
-        <v>2</v>
-      </c>
-      <c r="J16" s="12">
+      <c r="J22" s="14">
         <f t="shared" si="2"/>
         <v>43417</v>
       </c>
-      <c r="K16" s="39">
-        <v>3</v>
-      </c>
-      <c r="L16" s="13">
-        <f t="shared" si="3"/>
-        <v>43438</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="21" x14ac:dyDescent="0.25">
-      <c r="A17" s="49"/>
-      <c r="B17" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" s="9">
-        <v>43340</v>
-      </c>
-      <c r="E17" s="29">
+      <c r="K22" s="35">
         <v>8</v>
       </c>
-      <c r="F17" s="10">
-        <f t="shared" si="0"/>
-        <v>43396</v>
-      </c>
-      <c r="G17" s="33">
-        <v>2</v>
-      </c>
-      <c r="H17" s="11">
-        <f t="shared" si="1"/>
-        <v>43410</v>
-      </c>
-      <c r="I17" s="36">
-        <v>1</v>
-      </c>
-      <c r="J17" s="12">
-        <f t="shared" si="2"/>
-        <v>43417</v>
-      </c>
-      <c r="K17" s="39">
-        <v>3</v>
-      </c>
-      <c r="L17" s="13">
-        <f t="shared" si="3"/>
-        <v>43438</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="21" x14ac:dyDescent="0.25">
-      <c r="A18" s="50"/>
-      <c r="B18" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18" s="15">
-        <v>43242</v>
-      </c>
-      <c r="E18" s="30">
-        <v>3</v>
-      </c>
-      <c r="F18" s="16">
-        <f t="shared" si="0"/>
-        <v>43263</v>
-      </c>
-      <c r="G18" s="34">
-        <v>14</v>
-      </c>
-      <c r="H18" s="17">
-        <f t="shared" si="1"/>
-        <v>43361</v>
-      </c>
-      <c r="I18" s="37">
-        <v>14</v>
-      </c>
-      <c r="J18" s="18">
-        <f t="shared" si="2"/>
-        <v>43459</v>
-      </c>
-      <c r="K18" s="40">
-        <v>7</v>
-      </c>
-      <c r="L18" s="19">
-        <f t="shared" si="3"/>
-        <v>43508</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="21" x14ac:dyDescent="0.25">
-      <c r="A19" s="58" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" s="21">
-        <v>43396</v>
-      </c>
-      <c r="E19" s="31">
-        <v>2</v>
-      </c>
-      <c r="F19" s="22">
-        <f t="shared" si="0"/>
-        <v>43410</v>
-      </c>
-      <c r="G19" s="35">
-        <v>4</v>
-      </c>
-      <c r="H19" s="23">
-        <f t="shared" si="1"/>
-        <v>43438</v>
-      </c>
-      <c r="I19" s="38">
-        <v>4</v>
-      </c>
-      <c r="J19" s="24">
-        <f t="shared" si="2"/>
-        <v>43466</v>
-      </c>
-      <c r="K19" s="41">
-        <v>3</v>
-      </c>
-      <c r="L19" s="25">
-        <f t="shared" si="3"/>
-        <v>43487</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" ht="21" x14ac:dyDescent="0.25">
-      <c r="A20" s="50"/>
-      <c r="B20" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="D20" s="15">
-        <v>43396</v>
-      </c>
-      <c r="E20" s="30">
-        <v>2</v>
-      </c>
-      <c r="F20" s="16">
-        <f t="shared" si="0"/>
-        <v>43410</v>
-      </c>
-      <c r="G20" s="34">
-        <v>4</v>
-      </c>
-      <c r="H20" s="17">
-        <f t="shared" si="1"/>
-        <v>43438</v>
-      </c>
-      <c r="I20" s="37">
-        <v>4</v>
-      </c>
-      <c r="J20" s="18">
-        <f t="shared" si="2"/>
-        <v>43466</v>
-      </c>
-      <c r="K20" s="40">
-        <v>3</v>
-      </c>
-      <c r="L20" s="19">
-        <f t="shared" si="3"/>
-        <v>43487</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="21" x14ac:dyDescent="0.25">
-      <c r="A21" s="58" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" s="9">
-        <v>43242</v>
-      </c>
-      <c r="E21" s="29">
-        <v>3</v>
-      </c>
-      <c r="F21" s="10">
-        <f t="shared" si="0"/>
-        <v>43263</v>
-      </c>
-      <c r="G21" s="33">
-        <v>14</v>
-      </c>
-      <c r="H21" s="11">
-        <f t="shared" si="1"/>
-        <v>43361</v>
-      </c>
-      <c r="I21" s="36">
-        <v>7</v>
-      </c>
-      <c r="J21" s="12">
-        <f t="shared" si="2"/>
-        <v>43410</v>
-      </c>
-      <c r="K21" s="39">
-        <v>3</v>
-      </c>
-      <c r="L21" s="13">
-        <f t="shared" si="3"/>
-        <v>43431</v>
-      </c>
-      <c r="M21" s="4"/>
-    </row>
-    <row r="22" spans="1:13" ht="21" x14ac:dyDescent="0.25">
-      <c r="A22" s="50"/>
-      <c r="B22" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="15">
-        <v>43242</v>
-      </c>
-      <c r="E22" s="30">
-        <v>7</v>
-      </c>
-      <c r="F22" s="16">
-        <f t="shared" si="0"/>
-        <v>43291</v>
-      </c>
-      <c r="G22" s="34">
-        <v>11</v>
-      </c>
-      <c r="H22" s="17">
-        <f t="shared" si="1"/>
-        <v>43368</v>
-      </c>
-      <c r="I22" s="37">
-        <v>7</v>
-      </c>
-      <c r="J22" s="18">
-        <f t="shared" si="2"/>
-        <v>43417</v>
-      </c>
-      <c r="K22" s="40">
-        <v>8</v>
-      </c>
-      <c r="L22" s="19">
+      <c r="L22" s="15">
         <f t="shared" si="3"/>
         <v>43473</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="L25" s="7"/>
+    <row r="23" spans="1:13" ht="24.75" x14ac:dyDescent="0.4">
+      <c r="A23" s="65" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="66"/>
+      <c r="C23" s="66"/>
+      <c r="D23" s="66"/>
+      <c r="E23" s="67"/>
+      <c r="F23" s="68"/>
+      <c r="G23" s="67"/>
+      <c r="H23" s="68"/>
+      <c r="I23" s="67"/>
+      <c r="J23" s="68"/>
+      <c r="K23" s="67"/>
+      <c r="L23" s="69"/>
+    </row>
+    <row r="24" spans="1:13" ht="21" x14ac:dyDescent="0.45">
+      <c r="A24" s="73" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="73"/>
+      <c r="C24" s="73" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" s="73"/>
+      <c r="E24" s="73"/>
+      <c r="F24" s="73"/>
+      <c r="G24" s="73"/>
+      <c r="H24" s="73"/>
+      <c r="I24" s="73"/>
+      <c r="J24" s="73"/>
+      <c r="K24" s="73"/>
+      <c r="L24" s="70" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="21" x14ac:dyDescent="0.45">
+      <c r="A25" s="71" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="71"/>
+      <c r="C25" s="74" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" s="74"/>
+      <c r="E25" s="74"/>
+      <c r="F25" s="74"/>
+      <c r="G25" s="74"/>
+      <c r="H25" s="74"/>
+      <c r="I25" s="74"/>
+      <c r="J25" s="74"/>
+      <c r="K25" s="74"/>
+      <c r="L25" s="72">
+        <f>H4</f>
+        <v>43522</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="21" x14ac:dyDescent="0.45">
+      <c r="A26" s="71" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="71"/>
+      <c r="C26" s="74" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" s="74"/>
+      <c r="E26" s="74"/>
+      <c r="F26" s="74"/>
+      <c r="G26" s="74"/>
+      <c r="H26" s="74"/>
+      <c r="I26" s="74"/>
+      <c r="J26" s="74"/>
+      <c r="K26" s="74"/>
+      <c r="L26" s="72">
+        <f>MAX(L6:L22)</f>
+        <v>43578</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="21" x14ac:dyDescent="0.45">
+      <c r="A27" s="71" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" s="71"/>
+      <c r="C27" s="74" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" s="74"/>
+      <c r="E27" s="74"/>
+      <c r="F27" s="74"/>
+      <c r="G27" s="74"/>
+      <c r="H27" s="74"/>
+      <c r="I27" s="74"/>
+      <c r="J27" s="74"/>
+      <c r="K27" s="74"/>
+      <c r="L27" s="72">
+        <f>H5</f>
+        <v>43620</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="21" x14ac:dyDescent="0.45">
+      <c r="A28" s="71" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="71"/>
+      <c r="C28" s="74" t="s">
+        <v>58</v>
+      </c>
+      <c r="D28" s="74"/>
+      <c r="E28" s="74"/>
+      <c r="F28" s="74"/>
+      <c r="G28" s="74"/>
+      <c r="H28" s="74"/>
+      <c r="I28" s="74"/>
+      <c r="J28" s="74"/>
+      <c r="K28" s="74"/>
+      <c r="L28" s="72">
+        <f>J5</f>
+        <v>43648</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="21" x14ac:dyDescent="0.45">
+      <c r="A29" s="71" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" s="71"/>
+      <c r="C29" s="74" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29" s="74"/>
+      <c r="E29" s="74"/>
+      <c r="F29" s="74"/>
+      <c r="G29" s="74"/>
+      <c r="H29" s="74"/>
+      <c r="I29" s="74"/>
+      <c r="J29" s="74"/>
+      <c r="K29" s="74"/>
+      <c r="L29" s="72">
+        <f>L28+14</f>
+        <v>43662</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="21" x14ac:dyDescent="0.45">
+      <c r="A30" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" s="71"/>
+      <c r="C30" s="74" t="s">
+        <v>60</v>
+      </c>
+      <c r="D30" s="74"/>
+      <c r="E30" s="74"/>
+      <c r="F30" s="74"/>
+      <c r="G30" s="74"/>
+      <c r="H30" s="74"/>
+      <c r="I30" s="74"/>
+      <c r="J30" s="74"/>
+      <c r="K30" s="74"/>
+      <c r="L30" s="72">
+        <f>L29+14</f>
+        <v>43676</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="21" x14ac:dyDescent="0.45">
+      <c r="A31" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="B31" s="71"/>
+      <c r="C31" s="74" t="s">
+        <v>54</v>
+      </c>
+      <c r="D31" s="74"/>
+      <c r="E31" s="74"/>
+      <c r="F31" s="74"/>
+      <c r="G31" s="74"/>
+      <c r="H31" s="74"/>
+      <c r="I31" s="74"/>
+      <c r="J31" s="74"/>
+      <c r="K31" s="74"/>
+      <c r="L31" s="72">
+        <f>L30+14</f>
+        <v>43690</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="34">
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C25:K25"/>
+    <mergeCell ref="C29:K29"/>
+    <mergeCell ref="C30:K30"/>
+    <mergeCell ref="C31:K31"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:K26"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C28:K28"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="C27:K27"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="C24:K24"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K2:L2"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="E2:F2"/>
@@ -3725,20 +4603,244 @@
     <mergeCell ref="A10:A13"/>
     <mergeCell ref="A14:A18"/>
     <mergeCell ref="A4:A5"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.1" right="0.1" top="0.1" bottom="0.1" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" orientation="landscape" r:id="rId1"/>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="22" max="16383" man="1"/>
+  </rowBreaks>
   <ignoredErrors>
-    <ignoredError sqref="F4" formula="1"/>
+    <ignoredError sqref="F4 E5" formula="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9591EF12-12B5-44D5-911E-15D67C3B63C7}">
+  <dimension ref="A1:H31"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="str">
+        <f ca="1">_xlfn.CONCAT("Today: ", TEXT(TODAY(), "dd-mmm-yy"))</f>
+        <v>Today: 28-Oct-18</v>
+      </c>
+      <c r="G1" s="3">
+        <v>43816</v>
+      </c>
+      <c r="H1" s="2">
+        <f>INT(G1)</f>
+        <v>43816</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <f ca="1">TODAY()</f>
+        <v>43401</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <f ca="1">TODAY()</f>
+        <v>43401</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B5" t="str">
+        <f>Text!A25</f>
+        <v>EM Integration</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <f>Text!L25</f>
+        <v>43522</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <f>Text!L25</f>
+        <v>43522</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" t="str">
+        <f>Text!A26</f>
+        <v>EM Day in the Life Test</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <f>Text!L26</f>
+        <v>43578</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <f>Text!L26</f>
+        <v>43578</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" t="str">
+        <f>Text!A27</f>
+        <v>FU Integration</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <f>Text!L27</f>
+        <v>43620</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <f>Text!L27</f>
+        <v>43620</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="str">
+        <f>Text!A28</f>
+        <v>FU Day in the Life Test</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <f>Text!L28</f>
+        <v>43648</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <f>Text!L28</f>
+        <v>43648</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B21" t="str">
+        <f>Text!A29</f>
+        <v>FRR</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <f>Text!L29</f>
+        <v>43662</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <f>Text!L29</f>
+        <v>43662</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B25" t="str">
+        <f>Text!A30</f>
+        <v>MRR</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <f>Text!L30</f>
+        <v>43676</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <f>Text!L30</f>
+        <v>43676</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B29" t="str">
+        <f>Text!A31</f>
+        <v>ILC</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <f>Text!L31</f>
+        <v>43690</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <f>Text!L31</f>
+        <v>43690</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added battery test and licensing forms
</commit_message>
<xml_diff>
--- a/Native/CougSat1-Timeline.xlsx
+++ b/Native/CougSat1-Timeline.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bradley\Documents\GitHub\CougsInSpace\CougSat1-Readme\Native\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0253B5CE-F60E-4D0D-9E70-22E3D7193B87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD55C5DD-1133-47DE-84C3-34991F8D4522}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13425" activeTab="1" xr2:uid="{6C898573-EEE6-4764-A1E5-48C0D9787F59}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt" sheetId="8" r:id="rId1"/>
     <sheet name="Text" sheetId="7" r:id="rId2"/>
-    <sheet name="Gantt Lines" sheetId="9" state="hidden" r:id="rId3"/>
+    <sheet name="Gantt Lines" sheetId="9" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="Build">Text!$H$4:$H$21</definedName>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="56">
   <si>
     <t>Start</t>
   </si>
@@ -144,9 +144,6 @@
   </si>
   <si>
     <t>Last component of the milestone</t>
-  </si>
-  <si>
-    <t>V1.5.0</t>
   </si>
   <si>
     <t>Day in the Life Test</t>
@@ -223,6 +220,21 @@
   </si>
   <si>
     <t>Collection of tasks that mark important dates</t>
+  </si>
+  <si>
+    <t>Battery Qualification</t>
+  </si>
+  <si>
+    <t>Testing the batteries per the testing plan</t>
+  </si>
+  <si>
+    <t>All RF regulatory documents completed and being processed by regulatory bodies (FCC)</t>
+  </si>
+  <si>
+    <t>Radio Licensing Forms</t>
+  </si>
+  <si>
+    <t>V1.5.1</t>
   </si>
 </sst>
 </file>
@@ -1659,8 +1671,140 @@
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="9"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Gantt Lines'!$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Radio Licensing Forms</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="40000"/>
+                  <a:lumOff val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Gantt Lines'!$A$6:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>43891</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43891</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Gantt Lines'!$B$6:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-38E4-4B08-AFB0-72FBDC711CEC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Gantt Lines'!$B$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Battery Qualification</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Gantt Lines'!$A$10:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>43898</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43898</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Gantt Lines'!$B$10:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-38E4-4B08-AFB0-72FBDC711CEC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="2"/>
-          <c:order val="4"/>
+          <c:order val="6"/>
           <c:tx>
             <c:strRef>
               <c:f>'Gantt Lines'!$B$13</c:f>
@@ -1723,7 +1867,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
-          <c:order val="5"/>
+          <c:order val="7"/>
           <c:tx>
             <c:strRef>
               <c:f>'Gantt Lines'!$B$17</c:f>
@@ -1786,7 +1930,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="6"/>
-          <c:order val="6"/>
+          <c:order val="8"/>
           <c:tx>
             <c:strRef>
               <c:f>'Gantt Lines'!$B$21</c:f>
@@ -1849,7 +1993,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="7"/>
-          <c:order val="7"/>
+          <c:order val="9"/>
           <c:tx>
             <c:strRef>
               <c:f>'Gantt Lines'!$B$25</c:f>
@@ -1915,7 +2059,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="8"/>
-          <c:order val="8"/>
+          <c:order val="10"/>
           <c:tx>
             <c:strRef>
               <c:f>'Gantt Lines'!$B$29</c:f>
@@ -3111,10 +3255,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6795B2AF-B69F-4446-A3B6-FEFF9CA8AA9F}">
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3141,7 +3285,7 @@
       <c r="D1" s="57"/>
       <c r="E1" s="57"/>
       <c r="F1" s="25" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="G1" s="26"/>
       <c r="H1" s="25"/>
@@ -3185,7 +3329,7 @@
     </row>
     <row r="3" spans="1:12" s="3" customFormat="1" ht="29.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3" s="23" t="s">
         <v>29</v>
@@ -3551,7 +3695,7 @@
     <row r="13" spans="1:12" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A13" s="63"/>
       <c r="B13" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" s="31" t="s">
         <v>5</v>
@@ -3588,7 +3732,7 @@
     <row r="14" spans="1:12" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A14" s="63"/>
       <c r="B14" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C14" s="31" t="s">
         <v>5</v>
@@ -3625,7 +3769,7 @@
     <row r="15" spans="1:12" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A15" s="64"/>
       <c r="B15" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C15" s="43" t="s">
         <v>5</v>
@@ -3661,10 +3805,10 @@
     </row>
     <row r="16" spans="1:12" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A16" s="65" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C16" s="43" t="s">
         <v>7</v>
@@ -3700,7 +3844,7 @@
     <row r="17" spans="1:11" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A17" s="63"/>
       <c r="B17" s="49" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C17" s="49" t="s">
         <v>7</v>
@@ -3811,7 +3955,7 @@
     <row r="20" spans="1:11" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A20" s="63"/>
       <c r="B20" s="31" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C20" s="31" t="s">
         <v>7</v>
@@ -3848,7 +3992,7 @@
     <row r="21" spans="1:11" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A21" s="64"/>
       <c r="B21" s="43" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C21" s="43" t="s">
         <v>7</v>
@@ -3884,7 +4028,7 @@
     </row>
     <row r="22" spans="1:11" ht="23.25" x14ac:dyDescent="0.45">
       <c r="A22" s="56" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B22" s="57"/>
       <c r="C22" s="57"/>
@@ -3918,11 +4062,11 @@
     </row>
     <row r="24" spans="1:11" ht="20.25" x14ac:dyDescent="0.85">
       <c r="A24" s="54" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="B24" s="54"/>
       <c r="C24" s="55" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="D24" s="55"/>
       <c r="E24" s="55"/>
@@ -3932,17 +4076,16 @@
       <c r="I24" s="55"/>
       <c r="J24" s="55"/>
       <c r="K24" s="53">
-        <f>G4</f>
-        <v>43954</v>
+        <v>43891</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="20.25" x14ac:dyDescent="0.85">
       <c r="A25" s="54" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B25" s="54"/>
       <c r="C25" s="55" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D25" s="55"/>
       <c r="E25" s="55"/>
@@ -3952,17 +4095,16 @@
       <c r="I25" s="55"/>
       <c r="J25" s="55"/>
       <c r="K25" s="53">
-        <f>G4+7</f>
-        <v>43961</v>
+        <v>43898</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="20.25" x14ac:dyDescent="0.85">
       <c r="A26" s="54" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B26" s="54"/>
       <c r="C26" s="55" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D26" s="55"/>
       <c r="E26" s="55"/>
@@ -3972,17 +4114,17 @@
       <c r="I26" s="55"/>
       <c r="J26" s="55"/>
       <c r="K26" s="53">
-        <f>G16</f>
-        <v>43982</v>
+        <f>G4</f>
+        <v>43954</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="20.25" x14ac:dyDescent="0.85">
       <c r="A27" s="54" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B27" s="54"/>
       <c r="C27" s="55" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="D27" s="55"/>
       <c r="E27" s="55"/>
@@ -3992,13 +4134,13 @@
       <c r="I27" s="55"/>
       <c r="J27" s="55"/>
       <c r="K27" s="53">
-        <f>I16</f>
-        <v>43989</v>
+        <f>G4+7</f>
+        <v>43961</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="20.25" x14ac:dyDescent="0.85">
       <c r="A28" s="54" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B28" s="54"/>
       <c r="C28" s="55" t="s">
@@ -4012,6 +4154,46 @@
       <c r="I28" s="55"/>
       <c r="J28" s="55"/>
       <c r="K28" s="53">
+        <f>G16</f>
+        <v>43982</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="20.25" x14ac:dyDescent="0.85">
+      <c r="A29" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" s="54"/>
+      <c r="C29" s="55" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" s="55"/>
+      <c r="E29" s="55"/>
+      <c r="F29" s="55"/>
+      <c r="G29" s="55"/>
+      <c r="H29" s="55"/>
+      <c r="I29" s="55"/>
+      <c r="J29" s="55"/>
+      <c r="K29" s="53">
+        <f>I16</f>
+        <v>43989</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="20.25" x14ac:dyDescent="0.85">
+      <c r="A30" s="54" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30" s="54"/>
+      <c r="C30" s="55" t="s">
+        <v>47</v>
+      </c>
+      <c r="D30" s="55"/>
+      <c r="E30" s="55"/>
+      <c r="F30" s="55"/>
+      <c r="G30" s="55"/>
+      <c r="H30" s="55"/>
+      <c r="I30" s="55"/>
+      <c r="J30" s="55"/>
+      <c r="K30" s="53">
         <f>K16</f>
         <v>44010</v>
       </c>
@@ -4020,7 +4202,7 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B17:K21">
     <sortCondition descending="1" ref="K17:K21"/>
   </sortState>
-  <mergeCells count="23">
+  <mergeCells count="27">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="F3:G3"/>
@@ -4028,22 +4210,26 @@
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="A22:K22"/>
     <mergeCell ref="J2:K2"/>
-    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A27:B27"/>
     <mergeCell ref="C23:J23"/>
-    <mergeCell ref="C24:J24"/>
-    <mergeCell ref="C25:J25"/>
+    <mergeCell ref="C26:J26"/>
+    <mergeCell ref="C27:J27"/>
     <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A26:B26"/>
     <mergeCell ref="A4:A15"/>
     <mergeCell ref="A16:A21"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="H2:I2"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:J26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="C27:J27"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:J24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C25:J25"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="C28:J28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:J29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="C30:J30"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <conditionalFormatting sqref="D4:D21">
@@ -4054,6 +4240,9 @@
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.1" right="0.1" top="0.1" bottom="0.1" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" orientation="landscape" r:id="rId1"/>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="21" max="16383" man="1"/>
+  </rowBreaks>
 </worksheet>
 </file>
 
@@ -4062,7 +4251,7 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:B31"/>
+      <selection activeCell="A9" sqref="A9:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4114,30 +4303,66 @@
         <v>1</v>
       </c>
     </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="B5" t="str">
+        <f>Text!A24</f>
+        <v>Radio Licensing Forms</v>
+      </c>
+    </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A6" s="2"/>
+      <c r="A6" s="2">
+        <f>Text!K24</f>
+        <v>43891</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A7" s="2"/>
+      <c r="A7" s="2">
+        <f>Text!K24</f>
+        <v>43891</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="B9" t="str">
+        <f>Text!A25</f>
+        <v>Battery Qualification</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A10" s="2"/>
+      <c r="A10" s="2">
+        <f>Text!K25</f>
+        <v>43898</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A11" s="2"/>
+      <c r="A11" s="2">
+        <f>Text!K25</f>
+        <v>43898</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="2"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B13" t="str">
-        <f>Text!A24</f>
+        <f>Text!A26</f>
         <v>Flight Unit Integration</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="2">
-        <f>Text!K24</f>
+        <f>Text!K26</f>
         <v>43954</v>
       </c>
       <c r="B14">
@@ -4146,7 +4371,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="2">
-        <f>Text!K24</f>
+        <f>Text!K26</f>
         <v>43954</v>
       </c>
       <c r="B15">
@@ -4155,13 +4380,13 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B17" t="str">
-        <f>Text!A25</f>
+        <f>Text!A27</f>
         <v>Vibration Test</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" s="2">
-        <f>Text!K25</f>
+        <f>Text!K27</f>
         <v>43961</v>
       </c>
       <c r="B18">
@@ -4170,7 +4395,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" s="2">
-        <f>Text!K25</f>
+        <f>Text!K27</f>
         <v>43961</v>
       </c>
       <c r="B19">
@@ -4179,13 +4404,13 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B21" t="str">
-        <f>Text!A26</f>
+        <f>Text!A28</f>
         <v>Software Integration</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22" s="2">
-        <f>Text!K26</f>
+        <f>Text!K28</f>
         <v>43982</v>
       </c>
       <c r="B22">
@@ -4194,7 +4419,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" s="2">
-        <f>Text!K26</f>
+        <f>Text!K28</f>
         <v>43982</v>
       </c>
       <c r="B23">
@@ -4203,13 +4428,13 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B25" t="str">
-        <f>Text!A27</f>
+        <f>Text!A29</f>
         <v>Day in the Life Test</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A26" s="2">
-        <f>Text!K27</f>
+        <f>Text!K29</f>
         <v>43989</v>
       </c>
       <c r="B26">
@@ -4218,7 +4443,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A27" s="2">
-        <f>Text!K27</f>
+        <f>Text!K29</f>
         <v>43989</v>
       </c>
       <c r="B27">
@@ -4227,13 +4452,13 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B29" t="str">
-        <f>Text!A28</f>
+        <f>Text!A30</f>
         <v>Nanoracks Handover</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A30" s="2">
-        <f>Text!K28</f>
+        <f>Text!K30</f>
         <v>44010</v>
       </c>
       <c r="B30">
@@ -4242,7 +4467,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A31" s="2">
-        <f>Text!K28</f>
+        <f>Text!K30</f>
         <v>44010</v>
       </c>
       <c r="B31">

</xml_diff>

<commit_message>
Adjusted timeline for COVID
</commit_message>
<xml_diff>
--- a/Native/CougSat1-Timeline.xlsx
+++ b/Native/CougSat1-Timeline.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bradley\Documents\GitHub\CougsInSpace\CougSat1-Readme\Native\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bradley\Documents\Git\CougsInSpace\CougSat1-Readme\Native\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD55C5DD-1133-47DE-84C3-34991F8D4522}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0FEE232-7CEF-47E0-B7CE-E73DCB528B7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13425" activeTab="1" xr2:uid="{6C898573-EEE6-4764-A1E5-48C0D9787F59}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13875" activeTab="1" xr2:uid="{6C898573-EEE6-4764-A1E5-48C0D9787F59}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt" sheetId="8" r:id="rId1"/>
@@ -708,7 +708,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -739,9 +739,6 @@
     <xf numFmtId="165" fontId="7" fillId="11" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="7" fillId="9" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -791,9 +788,6 @@
     <xf numFmtId="165" fontId="7" fillId="14" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="14" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -851,18 +845,27 @@
     <xf numFmtId="0" fontId="7" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="7" fillId="14" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="166" fontId="7" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="16" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -873,6 +876,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1097,58 +1103,58 @@
                 <c:formatCode>[$-409]d\-mmm\-yy;@</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>43586</c:v>
+                  <c:v>44048</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43877</c:v>
+                  <c:v>44048</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43891</c:v>
+                  <c:v>44048</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43586</c:v>
+                  <c:v>44048</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43711</c:v>
+                  <c:v>44048</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43877</c:v>
+                  <c:v>44048</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43831</c:v>
+                  <c:v>44048</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43863</c:v>
+                  <c:v>44048</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43586</c:v>
+                  <c:v>44048</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43586</c:v>
+                  <c:v>44048</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43733</c:v>
+                  <c:v>44048</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43719</c:v>
+                  <c:v>44048</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43954</c:v>
+                  <c:v>44048</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43586</c:v>
+                  <c:v>44048</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43586</c:v>
+                  <c:v>44048</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43586</c:v>
+                  <c:v>44048</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43586</c:v>
+                  <c:v>44048</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>43586</c:v>
+                  <c:v>44048</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1262,58 +1268,58 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>368</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>49</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>312</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>187</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>28</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>46</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>35</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>312</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>333</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>172</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>67</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>28</c:v>
+                  <c:v>112</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>354</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>340</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>340</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>347</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>340</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1430,10 +1436,10 @@
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>28</c:v>
@@ -1442,37 +1448,37 @@
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>91</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>42</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>42</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>28</c:v>
@@ -1628,7 +1634,7 @@
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>21</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>14</c:v>
@@ -1835,10 +1841,10 @@
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>43954</c:v>
+                  <c:v>44146</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43954</c:v>
+                  <c:v>44146</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1898,10 +1904,10 @@
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>43961</c:v>
+                  <c:v>44153</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43961</c:v>
+                  <c:v>44153</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1961,10 +1967,10 @@
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>43982</c:v>
+                  <c:v>44160</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43982</c:v>
+                  <c:v>44160</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2027,10 +2033,10 @@
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>43989</c:v>
+                  <c:v>44181</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43989</c:v>
+                  <c:v>44181</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2093,10 +2099,10 @@
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>44010</c:v>
+                  <c:v>44195</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44010</c:v>
+                  <c:v>44195</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2189,8 +2195,7 @@
         <c:axId val="295186255"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="44027"/>
-          <c:min val="43863"/>
+          <c:min val="44048"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="t"/>
@@ -2929,7 +2934,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="12225338" cy="7196138"/>
+    <xdr:ext cx="12231624" cy="7202424"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -3257,8 +3262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6795B2AF-B69F-4446-A3B6-FEFF9CA8AA9F}">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3266,936 +3271,935 @@
     <col min="1" max="1" width="20.265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.59765625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15" style="48" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" style="46" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.59765625" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.59765625" style="17" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.59765625" style="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.59765625" style="17" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.1328125" style="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.1328125" style="17" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.3984375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="23.25" x14ac:dyDescent="0.45">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="25" t="s">
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="G1" s="26"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="26" t="s">
+      <c r="G1" s="25"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="69">
+      <c r="J1" s="71">
         <f>MAX(E4:K21)</f>
-        <v>44010</v>
-      </c>
-      <c r="K1" s="70"/>
+        <v>44195</v>
+      </c>
+      <c r="K1" s="72"/>
     </row>
     <row r="2" spans="1:12" s="3" customFormat="1" ht="20.25" x14ac:dyDescent="0.45">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="66" t="s">
+      <c r="F2" s="68" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="67"/>
-      <c r="H2" s="68" t="s">
+      <c r="G2" s="69"/>
+      <c r="H2" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="68"/>
-      <c r="J2" s="58" t="s">
+      <c r="I2" s="70"/>
+      <c r="J2" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="58"/>
+      <c r="K2" s="60"/>
     </row>
     <row r="3" spans="1:12" s="3" customFormat="1" ht="29.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="71" t="s">
+      <c r="F3" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="72"/>
-      <c r="H3" s="73" t="s">
+      <c r="G3" s="74"/>
+      <c r="H3" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="73"/>
-      <c r="J3" s="74" t="s">
+      <c r="I3" s="75"/>
+      <c r="J3" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="74"/>
-      <c r="L3" s="27"/>
+      <c r="K3" s="76"/>
+      <c r="L3" s="26"/>
     </row>
     <row r="4" spans="1:12" ht="20.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="62" t="s">
+      <c r="A4" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="45"/>
-      <c r="E4" s="34">
-        <v>43586</v>
-      </c>
-      <c r="F4" s="35">
-        <f t="shared" ref="F4:F21" si="0">(G4-E4)/7</f>
-        <v>52.571428571428569</v>
-      </c>
-      <c r="G4" s="36">
+      <c r="D4" s="43"/>
+      <c r="E4" s="32">
+        <v>44048</v>
+      </c>
+      <c r="F4" s="33">
+        <f t="shared" ref="F4:F16" si="0">(G4-E4)/7</f>
+        <v>14</v>
+      </c>
+      <c r="G4" s="34">
         <f>MAX(K5:K15)</f>
-        <v>43954</v>
-      </c>
-      <c r="H4" s="37">
+        <v>44146</v>
+      </c>
+      <c r="H4" s="35">
         <v>2</v>
       </c>
-      <c r="I4" s="38">
+      <c r="I4" s="36">
         <f t="shared" ref="I4:I21" si="1">G4+H4*7</f>
-        <v>43968</v>
-      </c>
-      <c r="J4" s="39">
+        <v>44160</v>
+      </c>
+      <c r="J4" s="37">
         <v>3</v>
       </c>
-      <c r="K4" s="40">
+      <c r="K4" s="38">
         <f t="shared" ref="K4:K15" si="2">I4+J4*7</f>
-        <v>43989</v>
+        <v>44181</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="20.25" x14ac:dyDescent="0.45">
-      <c r="A5" s="63"/>
+      <c r="A5" s="65"/>
       <c r="B5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="46" t="str">
+      <c r="D5" s="44" t="str">
         <f t="shared" ref="D5:D15" si="3">IF(K5=$G$4,"Critical Path","")</f>
-        <v>Critical Path</v>
-      </c>
-      <c r="E5" s="29">
-        <v>43877</v>
-      </c>
-      <c r="F5" s="15">
-        <f t="shared" si="0"/>
-        <v>7</v>
+        <v/>
+      </c>
+      <c r="E5" s="28">
+        <v>44048</v>
+      </c>
+      <c r="F5" s="14">
+        <v>4</v>
       </c>
       <c r="G5" s="5">
-        <v>43926</v>
-      </c>
-      <c r="H5" s="41">
-        <v>2</v>
+        <f>E5+F5*7</f>
+        <v>44076</v>
+      </c>
+      <c r="H5" s="39">
+        <v>4</v>
       </c>
       <c r="I5" s="6">
         <f t="shared" si="1"/>
-        <v>43940</v>
-      </c>
-      <c r="J5" s="42">
+        <v>44104</v>
+      </c>
+      <c r="J5" s="40">
         <v>2</v>
       </c>
       <c r="K5" s="7">
         <f t="shared" si="2"/>
-        <v>43954</v>
+        <v>44118</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="20.25" x14ac:dyDescent="0.45">
-      <c r="A6" s="63"/>
+      <c r="A6" s="65"/>
       <c r="B6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="46" t="str">
+      <c r="D6" s="44" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="E6" s="29">
-        <v>43891</v>
-      </c>
-      <c r="F6" s="15">
-        <f t="shared" si="0"/>
+      <c r="E6" s="28">
+        <v>44048</v>
+      </c>
+      <c r="F6" s="14">
         <v>4</v>
       </c>
       <c r="G6" s="5">
-        <v>43919</v>
-      </c>
-      <c r="H6" s="41">
-        <v>2</v>
+        <f t="shared" ref="G6:G14" si="4">E6+F6*7</f>
+        <v>44076</v>
+      </c>
+      <c r="H6" s="39">
+        <v>4</v>
       </c>
       <c r="I6" s="6">
         <f t="shared" si="1"/>
-        <v>43933</v>
-      </c>
-      <c r="J6" s="42">
+        <v>44104</v>
+      </c>
+      <c r="J6" s="40">
         <v>2</v>
       </c>
       <c r="K6" s="7">
         <f t="shared" si="2"/>
-        <v>43947</v>
+        <v>44118</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="20.25" x14ac:dyDescent="0.45">
-      <c r="A7" s="63"/>
+      <c r="A7" s="65"/>
       <c r="B7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="46" t="str">
+      <c r="D7" s="44" t="str">
+        <f t="shared" si="3"/>
+        <v>Critical Path</v>
+      </c>
+      <c r="E7" s="28">
+        <v>44048</v>
+      </c>
+      <c r="F7" s="14">
+        <v>8</v>
+      </c>
+      <c r="G7" s="5">
+        <f t="shared" si="4"/>
+        <v>44104</v>
+      </c>
+      <c r="H7" s="39">
+        <v>4</v>
+      </c>
+      <c r="I7" s="6">
+        <f t="shared" si="1"/>
+        <v>44132</v>
+      </c>
+      <c r="J7" s="40">
+        <v>2</v>
+      </c>
+      <c r="K7" s="7">
+        <f t="shared" si="2"/>
+        <v>44146</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="20.25" x14ac:dyDescent="0.45">
+      <c r="A8" s="65"/>
+      <c r="B8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="44" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="E7" s="29">
-        <v>43586</v>
-      </c>
-      <c r="F7" s="15">
-        <f t="shared" si="0"/>
-        <v>44.571428571428569</v>
-      </c>
-      <c r="G7" s="5">
-        <v>43898</v>
-      </c>
-      <c r="H7" s="41">
+      <c r="E8" s="28">
+        <v>44048</v>
+      </c>
+      <c r="F8" s="14">
         <v>4</v>
       </c>
-      <c r="I7" s="6">
-        <f t="shared" si="1"/>
-        <v>43926</v>
-      </c>
-      <c r="J7" s="42">
-        <v>2</v>
-      </c>
-      <c r="K7" s="7">
-        <f t="shared" si="2"/>
-        <v>43940</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="20.25" x14ac:dyDescent="0.45">
-      <c r="A8" s="63"/>
-      <c r="B8" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="46" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="E8" s="29">
-        <v>43711</v>
-      </c>
-      <c r="F8" s="15">
-        <f t="shared" si="0"/>
-        <v>26.714285714285715</v>
-      </c>
       <c r="G8" s="5">
-        <v>43898</v>
-      </c>
-      <c r="H8" s="41">
+        <f t="shared" si="4"/>
+        <v>44076</v>
+      </c>
+      <c r="H8" s="39">
         <v>2</v>
       </c>
       <c r="I8" s="6">
         <f t="shared" si="1"/>
-        <v>43912</v>
-      </c>
-      <c r="J8" s="42">
+        <v>44090</v>
+      </c>
+      <c r="J8" s="40">
         <v>2</v>
       </c>
       <c r="K8" s="7">
         <f t="shared" si="2"/>
-        <v>43926</v>
+        <v>44104</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="20.25" x14ac:dyDescent="0.45">
-      <c r="A9" s="63"/>
+      <c r="A9" s="65"/>
       <c r="B9" s="4" t="str">
         <f>"+X Panel V1.1"</f>
         <v>+X Panel V1.1</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="46" t="str">
+      <c r="D9" s="44" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="E9" s="29">
-        <v>43877</v>
-      </c>
-      <c r="F9" s="15">
-        <f t="shared" si="0"/>
-        <v>4</v>
+      <c r="E9" s="28">
+        <v>44048</v>
+      </c>
+      <c r="F9" s="14">
+        <v>8</v>
       </c>
       <c r="G9" s="5">
-        <v>43905</v>
-      </c>
-      <c r="H9" s="41">
-        <v>1</v>
+        <f t="shared" si="4"/>
+        <v>44104</v>
+      </c>
+      <c r="H9" s="39">
+        <v>2</v>
       </c>
       <c r="I9" s="6">
         <f t="shared" si="1"/>
-        <v>43912</v>
-      </c>
-      <c r="J9" s="42">
+        <v>44118</v>
+      </c>
+      <c r="J9" s="40">
         <v>2</v>
       </c>
       <c r="K9" s="7">
         <f t="shared" si="2"/>
-        <v>43926</v>
+        <v>44132</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="20.25" x14ac:dyDescent="0.45">
-      <c r="A10" s="63"/>
+      <c r="A10" s="65"/>
       <c r="B10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="31" t="s">
+      <c r="C10" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="46" t="str">
+      <c r="D10" s="44" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="E10" s="29">
-        <v>43831</v>
-      </c>
-      <c r="F10" s="15">
-        <f t="shared" si="0"/>
-        <v>6.5714285714285712</v>
+      <c r="E10" s="28">
+        <v>44048</v>
+      </c>
+      <c r="F10" s="14">
+        <v>4</v>
       </c>
       <c r="G10" s="5">
-        <v>43877</v>
-      </c>
-      <c r="H10" s="41">
-        <v>4</v>
+        <f t="shared" si="4"/>
+        <v>44076</v>
+      </c>
+      <c r="H10" s="39">
+        <v>6</v>
       </c>
       <c r="I10" s="6">
         <f t="shared" si="1"/>
-        <v>43905</v>
-      </c>
-      <c r="J10" s="42">
+        <v>44118</v>
+      </c>
+      <c r="J10" s="40">
         <v>2</v>
       </c>
       <c r="K10" s="7">
         <f t="shared" si="2"/>
-        <v>43919</v>
+        <v>44132</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="20.25" x14ac:dyDescent="0.45">
-      <c r="A11" s="63"/>
+      <c r="A11" s="65"/>
       <c r="B11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="46" t="str">
+      <c r="D11" s="44" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="E11" s="29">
-        <v>43863</v>
-      </c>
-      <c r="F11" s="15">
-        <f t="shared" si="0"/>
-        <v>5</v>
+      <c r="E11" s="28">
+        <v>44048</v>
+      </c>
+      <c r="F11" s="14">
+        <v>2</v>
       </c>
       <c r="G11" s="5">
-        <v>43898</v>
-      </c>
-      <c r="H11" s="41">
-        <v>1</v>
+        <f t="shared" si="4"/>
+        <v>44062</v>
+      </c>
+      <c r="H11" s="39">
+        <v>2</v>
       </c>
       <c r="I11" s="6">
         <f t="shared" si="1"/>
-        <v>43905</v>
-      </c>
-      <c r="J11" s="42">
+        <v>44076</v>
+      </c>
+      <c r="J11" s="40">
         <v>2</v>
       </c>
       <c r="K11" s="7">
         <f t="shared" si="2"/>
-        <v>43919</v>
+        <v>44090</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="20.25" x14ac:dyDescent="0.45">
-      <c r="A12" s="63"/>
-      <c r="B12" s="43" t="str">
+      <c r="A12" s="65"/>
+      <c r="B12" s="41" t="str">
         <f>"-Z Panel V1.0"</f>
         <v>-Z Panel V1.0</v>
       </c>
-      <c r="C12" s="43" t="s">
+      <c r="C12" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="47" t="str">
+      <c r="D12" s="45" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="E12" s="28">
-        <v>43586</v>
-      </c>
-      <c r="F12" s="16">
-        <f t="shared" si="0"/>
-        <v>44.571428571428569</v>
+      <c r="E12" s="27">
+        <v>44048</v>
+      </c>
+      <c r="F12" s="15">
+        <v>4</v>
       </c>
       <c r="G12" s="9">
-        <v>43898</v>
-      </c>
-      <c r="H12" s="32">
-        <v>1</v>
+        <f>E12+F12*7</f>
+        <v>44076</v>
+      </c>
+      <c r="H12" s="30">
+        <v>2</v>
       </c>
       <c r="I12" s="10">
         <f t="shared" si="1"/>
-        <v>43905</v>
-      </c>
-      <c r="J12" s="19">
+        <v>44090</v>
+      </c>
+      <c r="J12" s="18">
         <v>2</v>
       </c>
       <c r="K12" s="11">
         <f t="shared" si="2"/>
-        <v>43919</v>
+        <v>44104</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="20.25" x14ac:dyDescent="0.45">
-      <c r="A13" s="63"/>
+      <c r="A13" s="65"/>
       <c r="B13" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="31" t="s">
+      <c r="C13" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="46" t="str">
+      <c r="D13" s="44" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="E13" s="29">
-        <v>43586</v>
-      </c>
-      <c r="F13" s="15">
-        <f t="shared" si="0"/>
-        <v>47.571428571428569</v>
+      <c r="E13" s="28">
+        <v>44048</v>
+      </c>
+      <c r="F13" s="14">
+        <v>6</v>
       </c>
       <c r="G13" s="5">
-        <v>43919</v>
-      </c>
-      <c r="H13" s="41">
-        <v>2</v>
+        <f t="shared" si="4"/>
+        <v>44090</v>
+      </c>
+      <c r="H13" s="39">
+        <v>4</v>
       </c>
       <c r="I13" s="6">
         <f t="shared" si="1"/>
-        <v>43933</v>
-      </c>
-      <c r="J13" s="44">
+        <v>44118</v>
+      </c>
+      <c r="J13" s="42">
         <v>2</v>
       </c>
       <c r="K13" s="7">
         <f t="shared" si="2"/>
-        <v>43947</v>
+        <v>44132</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="20.25" x14ac:dyDescent="0.45">
-      <c r="A14" s="63"/>
+      <c r="A14" s="65"/>
       <c r="B14" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="46" t="str">
+      <c r="D14" s="44" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="E14" s="29">
-        <v>43733</v>
-      </c>
-      <c r="F14" s="15">
-        <f t="shared" si="0"/>
-        <v>24.571428571428573</v>
+      <c r="E14" s="28">
+        <v>44048</v>
+      </c>
+      <c r="F14" s="14">
+        <v>8</v>
       </c>
       <c r="G14" s="5">
-        <v>43905</v>
-      </c>
-      <c r="H14" s="41">
+        <f t="shared" si="4"/>
+        <v>44104</v>
+      </c>
+      <c r="H14" s="39">
         <v>2</v>
       </c>
       <c r="I14" s="6">
         <f t="shared" si="1"/>
-        <v>43919</v>
-      </c>
-      <c r="J14" s="42">
+        <v>44118</v>
+      </c>
+      <c r="J14" s="40">
         <v>2</v>
       </c>
       <c r="K14" s="7">
         <f t="shared" si="2"/>
-        <v>43933</v>
+        <v>44132</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="20.25" x14ac:dyDescent="0.45">
-      <c r="A15" s="64"/>
+      <c r="A15" s="66"/>
       <c r="B15" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="43" t="s">
+      <c r="C15" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="47" t="str">
+      <c r="D15" s="45" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="E15" s="28">
-        <v>43719</v>
-      </c>
-      <c r="F15" s="16">
-        <f t="shared" si="0"/>
-        <v>9.5714285714285712</v>
+      <c r="E15" s="27">
+        <v>44048</v>
+      </c>
+      <c r="F15" s="15">
+        <v>4</v>
       </c>
       <c r="G15" s="9">
-        <v>43786</v>
-      </c>
-      <c r="H15" s="32">
-        <v>13</v>
+        <f>E15+F15*7</f>
+        <v>44076</v>
+      </c>
+      <c r="H15" s="30">
+        <v>2</v>
       </c>
       <c r="I15" s="10">
         <f t="shared" si="1"/>
-        <v>43877</v>
-      </c>
-      <c r="J15" s="19">
+        <v>44090</v>
+      </c>
+      <c r="J15" s="18">
         <v>2</v>
       </c>
       <c r="K15" s="11">
         <f t="shared" si="2"/>
-        <v>43891</v>
+        <v>44104</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="20.25" x14ac:dyDescent="0.45">
-      <c r="A16" s="65" t="s">
+      <c r="A16" s="67" t="s">
         <v>39</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="43" t="s">
+      <c r="C16" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="47"/>
-      <c r="E16" s="28">
-        <f>G4</f>
-        <v>43954</v>
-      </c>
-      <c r="F16" s="16">
+      <c r="D16" s="45"/>
+      <c r="E16" s="27">
+        <v>44048</v>
+      </c>
+      <c r="F16" s="15">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="G16" s="9">
+        <v>16</v>
+      </c>
+      <c r="G16" s="5">
         <f>MAX(K17:K21)</f>
-        <v>43982</v>
-      </c>
-      <c r="H16" s="32">
-        <v>1</v>
+        <v>44160</v>
+      </c>
+      <c r="H16" s="30">
+        <v>3</v>
       </c>
       <c r="I16" s="10">
         <f t="shared" si="1"/>
-        <v>43989</v>
-      </c>
-      <c r="J16" s="19">
-        <v>3</v>
+        <v>44181</v>
+      </c>
+      <c r="J16" s="18">
+        <v>2</v>
       </c>
       <c r="K16" s="11">
-        <f t="shared" ref="K16" si="4">I16+J16*7</f>
-        <v>44010</v>
+        <f t="shared" ref="K16" si="5">I16+J16*7</f>
+        <v>44195</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="20.25" x14ac:dyDescent="0.45">
-      <c r="A17" s="63"/>
-      <c r="B17" s="49" t="s">
+      <c r="A17" s="65"/>
+      <c r="B17" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="49" t="s">
+      <c r="C17" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="46" t="str">
+      <c r="D17" s="44" t="str">
         <f>IF(K17=$G$16,"Critical Path","")</f>
         <v>Critical Path</v>
       </c>
-      <c r="E17" s="30">
-        <v>43586</v>
-      </c>
-      <c r="F17" s="17">
-        <f t="shared" si="0"/>
-        <v>50.571428571428569</v>
-      </c>
-      <c r="G17" s="12">
-        <v>43940</v>
+      <c r="E17" s="28">
+        <v>44048</v>
+      </c>
+      <c r="F17" s="16">
+        <v>10</v>
+      </c>
+      <c r="G17" s="53">
+        <f>E17+F17*7</f>
+        <v>44118</v>
       </c>
       <c r="H17" s="50">
         <v>4</v>
       </c>
-      <c r="I17" s="13">
+      <c r="I17" s="12">
         <f t="shared" si="1"/>
-        <v>43968</v>
-      </c>
-      <c r="J17" s="20">
+        <v>44146</v>
+      </c>
+      <c r="J17" s="19">
         <v>2</v>
       </c>
-      <c r="K17" s="14">
+      <c r="K17" s="13">
         <f>I17+J17*7</f>
-        <v>43982</v>
+        <v>44160</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="20.25" x14ac:dyDescent="0.45">
-      <c r="A18" s="63"/>
-      <c r="B18" s="31" t="s">
+      <c r="A18" s="65"/>
+      <c r="B18" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="31" t="s">
+      <c r="C18" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="46" t="str">
+      <c r="D18" s="44" t="str">
         <f>IF(K18=$G$16,"Critical Path","")</f>
         <v>Critical Path</v>
       </c>
-      <c r="E18" s="29">
-        <v>43586</v>
-      </c>
-      <c r="F18" s="15">
-        <f t="shared" si="0"/>
-        <v>48.571428571428569</v>
-      </c>
-      <c r="G18" s="5">
-        <v>43926</v>
-      </c>
-      <c r="H18" s="51">
-        <v>6</v>
+      <c r="E18" s="28">
+        <v>44048</v>
+      </c>
+      <c r="F18" s="14">
+        <v>10</v>
+      </c>
+      <c r="G18" s="52">
+        <f>E18+F18*7</f>
+        <v>44118</v>
+      </c>
+      <c r="H18" s="39">
+        <v>4</v>
       </c>
       <c r="I18" s="6">
         <f t="shared" si="1"/>
-        <v>43968</v>
-      </c>
-      <c r="J18" s="42">
+        <v>44146</v>
+      </c>
+      <c r="J18" s="40">
         <v>2</v>
       </c>
       <c r="K18" s="7">
         <f>I18+J18*7</f>
-        <v>43982</v>
+        <v>44160</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="20.25" x14ac:dyDescent="0.45">
-      <c r="A19" s="63"/>
-      <c r="B19" s="31" t="s">
+      <c r="A19" s="65"/>
+      <c r="B19" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="31" t="s">
+      <c r="C19" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="46" t="str">
+      <c r="D19" s="44" t="str">
         <f>IF(K19=$G$16,"Critical Path","")</f>
         <v>Critical Path</v>
       </c>
-      <c r="E19" s="29">
-        <v>43586</v>
-      </c>
-      <c r="F19" s="15">
-        <f t="shared" si="0"/>
-        <v>48.571428571428569</v>
-      </c>
-      <c r="G19" s="5">
-        <v>43926</v>
-      </c>
-      <c r="H19" s="51">
-        <v>6</v>
+      <c r="E19" s="28">
+        <v>44048</v>
+      </c>
+      <c r="F19" s="14">
+        <v>10</v>
+      </c>
+      <c r="G19" s="52">
+        <f>E19+F19*7</f>
+        <v>44118</v>
+      </c>
+      <c r="H19" s="39">
+        <v>4</v>
       </c>
       <c r="I19" s="6">
         <f t="shared" si="1"/>
-        <v>43968</v>
-      </c>
-      <c r="J19" s="42">
+        <v>44146</v>
+      </c>
+      <c r="J19" s="40">
         <v>2</v>
       </c>
       <c r="K19" s="7">
         <f>I19+J19*7</f>
-        <v>43982</v>
+        <v>44160</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="20.25" x14ac:dyDescent="0.45">
-      <c r="A20" s="63"/>
-      <c r="B20" s="31" t="s">
+      <c r="A20" s="65"/>
+      <c r="B20" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="31" t="s">
+      <c r="C20" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="46" t="str">
+      <c r="D20" s="44" t="str">
         <f>IF(K20=$G$16,"Critical Path","")</f>
-        <v/>
-      </c>
-      <c r="E20" s="29">
-        <v>43586</v>
-      </c>
-      <c r="F20" s="15">
-        <f t="shared" si="0"/>
-        <v>49.571428571428569</v>
-      </c>
-      <c r="G20" s="5">
-        <v>43933</v>
-      </c>
-      <c r="H20" s="51">
+        <v>Critical Path</v>
+      </c>
+      <c r="E20" s="28">
+        <v>44048</v>
+      </c>
+      <c r="F20" s="14">
+        <v>10</v>
+      </c>
+      <c r="G20" s="52">
+        <f>E20+F20*7</f>
+        <v>44118</v>
+      </c>
+      <c r="H20" s="39">
         <v>4</v>
       </c>
       <c r="I20" s="6">
         <f t="shared" si="1"/>
-        <v>43961</v>
-      </c>
-      <c r="J20" s="42">
+        <v>44146</v>
+      </c>
+      <c r="J20" s="40">
         <v>2</v>
       </c>
       <c r="K20" s="7">
         <f>I20+J20*7</f>
-        <v>43975</v>
+        <v>44160</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="20.25" x14ac:dyDescent="0.45">
-      <c r="A21" s="64"/>
-      <c r="B21" s="43" t="s">
+      <c r="A21" s="66"/>
+      <c r="B21" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="43" t="s">
+      <c r="C21" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="52" t="str">
+      <c r="D21" s="48" t="str">
         <f>IF(K21=$G$16,"Critical Path","")</f>
-        <v/>
+        <v>Critical Path</v>
       </c>
       <c r="E21" s="28">
-        <v>43586</v>
-      </c>
-      <c r="F21" s="16">
-        <f t="shared" si="0"/>
-        <v>48.571428571428569</v>
-      </c>
-      <c r="G21" s="9">
-        <v>43926</v>
-      </c>
-      <c r="H21" s="32">
+        <v>44048</v>
+      </c>
+      <c r="F21" s="15">
+        <v>10</v>
+      </c>
+      <c r="G21" s="54">
+        <f>E21+F21*7</f>
+        <v>44118</v>
+      </c>
+      <c r="H21" s="51">
         <v>4</v>
       </c>
       <c r="I21" s="10">
         <f t="shared" si="1"/>
-        <v>43954</v>
-      </c>
-      <c r="J21" s="19">
+        <v>44146</v>
+      </c>
+      <c r="J21" s="18">
         <v>2</v>
       </c>
       <c r="K21" s="11">
         <f>I21+J21*7</f>
-        <v>43968</v>
+        <v>44160</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="23.25" x14ac:dyDescent="0.45">
-      <c r="A22" s="56" t="s">
+      <c r="A22" s="57" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="57"/>
-      <c r="C22" s="57"/>
-      <c r="D22" s="57"/>
-      <c r="E22" s="57"/>
-      <c r="F22" s="57"/>
-      <c r="G22" s="57"/>
-      <c r="H22" s="57"/>
-      <c r="I22" s="57"/>
-      <c r="J22" s="57"/>
-      <c r="K22" s="57"/>
+      <c r="B22" s="58"/>
+      <c r="C22" s="58"/>
+      <c r="D22" s="58"/>
+      <c r="E22" s="58"/>
+      <c r="F22" s="58"/>
+      <c r="G22" s="59"/>
+      <c r="H22" s="58"/>
+      <c r="I22" s="58"/>
+      <c r="J22" s="58"/>
+      <c r="K22" s="58"/>
     </row>
     <row r="23" spans="1:11" ht="20.25" x14ac:dyDescent="0.45">
-      <c r="A23" s="59" t="s">
+      <c r="A23" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="61"/>
-      <c r="C23" s="59" t="s">
+      <c r="B23" s="63"/>
+      <c r="C23" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="D23" s="60"/>
-      <c r="E23" s="60"/>
-      <c r="F23" s="60"/>
-      <c r="G23" s="60"/>
-      <c r="H23" s="60"/>
-      <c r="I23" s="60"/>
-      <c r="J23" s="61"/>
-      <c r="K23" s="22" t="s">
+      <c r="D23" s="62"/>
+      <c r="E23" s="62"/>
+      <c r="F23" s="62"/>
+      <c r="G23" s="62"/>
+      <c r="H23" s="62"/>
+      <c r="I23" s="62"/>
+      <c r="J23" s="63"/>
+      <c r="K23" s="21" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="20.25" x14ac:dyDescent="0.85">
-      <c r="A24" s="54" t="s">
+      <c r="A24" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="B24" s="54"/>
-      <c r="C24" s="55" t="s">
+      <c r="B24" s="55"/>
+      <c r="C24" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="D24" s="55"/>
-      <c r="E24" s="55"/>
-      <c r="F24" s="55"/>
-      <c r="G24" s="55"/>
-      <c r="H24" s="55"/>
-      <c r="I24" s="55"/>
-      <c r="J24" s="55"/>
-      <c r="K24" s="53">
+      <c r="D24" s="56"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="56"/>
+      <c r="G24" s="56"/>
+      <c r="H24" s="56"/>
+      <c r="I24" s="56"/>
+      <c r="J24" s="56"/>
+      <c r="K24" s="49">
         <v>43891</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="20.25" x14ac:dyDescent="0.85">
-      <c r="A25" s="54" t="s">
+      <c r="A25" s="55" t="s">
         <v>51</v>
       </c>
-      <c r="B25" s="54"/>
-      <c r="C25" s="55" t="s">
+      <c r="B25" s="55"/>
+      <c r="C25" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="D25" s="55"/>
-      <c r="E25" s="55"/>
-      <c r="F25" s="55"/>
-      <c r="G25" s="55"/>
-      <c r="H25" s="55"/>
-      <c r="I25" s="55"/>
-      <c r="J25" s="55"/>
-      <c r="K25" s="53">
+      <c r="D25" s="56"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="56"/>
+      <c r="G25" s="56"/>
+      <c r="H25" s="56"/>
+      <c r="I25" s="56"/>
+      <c r="J25" s="56"/>
+      <c r="K25" s="49">
         <v>43898</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="20.25" x14ac:dyDescent="0.85">
-      <c r="A26" s="54" t="s">
+      <c r="A26" s="55" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="54"/>
-      <c r="C26" s="55" t="s">
+      <c r="B26" s="55"/>
+      <c r="C26" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="D26" s="55"/>
-      <c r="E26" s="55"/>
-      <c r="F26" s="55"/>
-      <c r="G26" s="55"/>
-      <c r="H26" s="55"/>
-      <c r="I26" s="55"/>
-      <c r="J26" s="55"/>
-      <c r="K26" s="53">
+      <c r="D26" s="56"/>
+      <c r="E26" s="56"/>
+      <c r="F26" s="56"/>
+      <c r="G26" s="56"/>
+      <c r="H26" s="56"/>
+      <c r="I26" s="56"/>
+      <c r="J26" s="56"/>
+      <c r="K26" s="49">
         <f>G4</f>
-        <v>43954</v>
+        <v>44146</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="20.25" x14ac:dyDescent="0.85">
-      <c r="A27" s="54" t="s">
+      <c r="A27" s="55" t="s">
         <v>41</v>
       </c>
-      <c r="B27" s="54"/>
-      <c r="C27" s="55" t="s">
+      <c r="B27" s="55"/>
+      <c r="C27" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="55"/>
-      <c r="E27" s="55"/>
-      <c r="F27" s="55"/>
-      <c r="G27" s="55"/>
-      <c r="H27" s="55"/>
-      <c r="I27" s="55"/>
-      <c r="J27" s="55"/>
-      <c r="K27" s="53">
+      <c r="D27" s="56"/>
+      <c r="E27" s="56"/>
+      <c r="F27" s="56"/>
+      <c r="G27" s="56"/>
+      <c r="H27" s="56"/>
+      <c r="I27" s="56"/>
+      <c r="J27" s="56"/>
+      <c r="K27" s="49">
         <f>G4+7</f>
-        <v>43961</v>
+        <v>44153</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="20.25" x14ac:dyDescent="0.85">
-      <c r="A28" s="54" t="s">
+      <c r="A28" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="B28" s="54"/>
-      <c r="C28" s="55" t="s">
+      <c r="B28" s="55"/>
+      <c r="C28" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="D28" s="55"/>
-      <c r="E28" s="55"/>
-      <c r="F28" s="55"/>
-      <c r="G28" s="55"/>
-      <c r="H28" s="55"/>
-      <c r="I28" s="55"/>
-      <c r="J28" s="55"/>
-      <c r="K28" s="53">
+      <c r="D28" s="56"/>
+      <c r="E28" s="56"/>
+      <c r="F28" s="56"/>
+      <c r="G28" s="56"/>
+      <c r="H28" s="56"/>
+      <c r="I28" s="56"/>
+      <c r="J28" s="56"/>
+      <c r="K28" s="49">
         <f>G16</f>
-        <v>43982</v>
+        <v>44160</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="20.25" x14ac:dyDescent="0.85">
-      <c r="A29" s="54" t="s">
+      <c r="A29" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="54"/>
-      <c r="C29" s="55" t="s">
+      <c r="B29" s="55"/>
+      <c r="C29" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="D29" s="55"/>
-      <c r="E29" s="55"/>
-      <c r="F29" s="55"/>
-      <c r="G29" s="55"/>
-      <c r="H29" s="55"/>
-      <c r="I29" s="55"/>
-      <c r="J29" s="55"/>
-      <c r="K29" s="53">
+      <c r="D29" s="56"/>
+      <c r="E29" s="56"/>
+      <c r="F29" s="56"/>
+      <c r="G29" s="56"/>
+      <c r="H29" s="56"/>
+      <c r="I29" s="56"/>
+      <c r="J29" s="56"/>
+      <c r="K29" s="49">
         <f>I16</f>
-        <v>43989</v>
+        <v>44181</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="20.25" x14ac:dyDescent="0.85">
-      <c r="A30" s="54" t="s">
+      <c r="A30" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="B30" s="54"/>
-      <c r="C30" s="55" t="s">
+      <c r="B30" s="55"/>
+      <c r="C30" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="D30" s="55"/>
-      <c r="E30" s="55"/>
-      <c r="F30" s="55"/>
-      <c r="G30" s="55"/>
-      <c r="H30" s="55"/>
-      <c r="I30" s="55"/>
-      <c r="J30" s="55"/>
-      <c r="K30" s="53">
+      <c r="D30" s="56"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="56"/>
+      <c r="G30" s="56"/>
+      <c r="H30" s="56"/>
+      <c r="I30" s="56"/>
+      <c r="J30" s="56"/>
+      <c r="K30" s="49">
         <f>K16</f>
-        <v>44010</v>
+        <v>44195</v>
       </c>
     </row>
   </sheetData>
@@ -4251,7 +4255,7 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:B11"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4271,24 +4275,24 @@
     <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B1" s="1" t="str">
         <f ca="1">_xlfn.CONCAT("Today: ", TEXT(TODAY(), "dd-mmm-yy"))</f>
-        <v>Today: 14-Feb-20</v>
+        <v>Today: 04-Jun-20</v>
       </c>
       <c r="G1" s="2">
-        <v>43863</v>
+        <v>44048</v>
       </c>
       <c r="H1">
         <f>INT(G1)</f>
-        <v>43863</v>
+        <v>44048</v>
       </c>
       <c r="I1">
         <f>H1+28</f>
-        <v>43891</v>
+        <v>44076</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <f ca="1">TODAY()</f>
-        <v>43875</v>
+        <v>43986</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -4297,7 +4301,7 @@
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <f ca="1">TODAY()</f>
-        <v>43875</v>
+        <v>43986</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -4363,7 +4367,7 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="2">
         <f>Text!K26</f>
-        <v>43954</v>
+        <v>44146</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -4372,7 +4376,7 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="2">
         <f>Text!K26</f>
-        <v>43954</v>
+        <v>44146</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -4387,7 +4391,7 @@
     <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" s="2">
         <f>Text!K27</f>
-        <v>43961</v>
+        <v>44153</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -4396,7 +4400,7 @@
     <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" s="2">
         <f>Text!K27</f>
-        <v>43961</v>
+        <v>44153</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -4411,7 +4415,7 @@
     <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22" s="2">
         <f>Text!K28</f>
-        <v>43982</v>
+        <v>44160</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -4420,7 +4424,7 @@
     <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" s="2">
         <f>Text!K28</f>
-        <v>43982</v>
+        <v>44160</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -4435,7 +4439,7 @@
     <row r="26" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A26" s="2">
         <f>Text!K29</f>
-        <v>43989</v>
+        <v>44181</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -4444,7 +4448,7 @@
     <row r="27" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A27" s="2">
         <f>Text!K29</f>
-        <v>43989</v>
+        <v>44181</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -4459,7 +4463,7 @@
     <row r="30" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A30" s="2">
         <f>Text!K30</f>
-        <v>44010</v>
+        <v>44195</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -4468,7 +4472,7 @@
     <row r="31" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A31" s="2">
         <f>Text!K30</f>
-        <v>44010</v>
+        <v>44195</v>
       </c>
       <c r="B31">
         <v>1</v>

</xml_diff>